<commit_message>
v1.2 An error message will be displayed if the article body exceeds 1000 words
</commit_message>
<xml_diff>
--- a/LH_ASSUMPTIONS/LH_SRS_ASSUMPTIONS.xlsx
+++ b/LH_ASSUMPTIONS/LH_SRS_ASSUMPTIONS.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="LH_SRS_ASSUMPTIONS" sheetId="2" r:id="rId1"/>
     <sheet name="Version Histroy" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -96,12 +101,40 @@
   </si>
   <si>
     <t>Gehad Ashry</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>LH-SRS-ASSUMP-002</t>
+  </si>
+  <si>
+    <t>SRS-PUB-004</t>
+  </si>
+  <si>
+    <t>An error message will be displayed if the article body exceeds 1000 words</t>
+  </si>
+  <si>
+    <t>The system will not show an error message if the article exceeds 1000 words, and the user will not be informed that the article cannot be submitted due to the word limit being exceeded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I made an assumption on the error message that will be shown if the user tries to submit an article that exceeds 1000 words: ["Exceeds 1000 words"].
+</t>
+  </si>
+  <si>
+    <t>V1.2</t>
+  </si>
+  <si>
+    <t>Hala  Eldaly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -176,11 +209,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,7 +546,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,7 +557,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +571,7 @@
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -570,38 +606,66 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+    <row r="2" spans="1:10" s="6" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <f ca="1">TODAY()</f>
-        <v>45769</v>
-      </c>
-      <c r="B2" s="6" t="s">
+        <v>45773</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:10" s="6" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>45773</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -675,7 +739,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +776,7 @@
       </c>
       <c r="D2" s="4">
         <f ca="1">TODAY()</f>
-        <v>45769</v>
+        <v>45773</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -727,14 +791,22 @@
       </c>
       <c r="D3" s="4">
         <f ca="1">TODAY()</f>
-        <v>45769</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45773</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>

</xml_diff>